<commit_message>
Added on Aug 21
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/sfdcTestData.xlsx
+++ b/src/main/resources/TestData/sfdcTestData.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athiranihit/Desktop/Eclipse_Project1/sfdc.org.project/src/main/resources/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athiranihit/Desktop/Aug21/sfdc.org.project/src/main/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F70ADD8-DB85-584B-B676-0232316430F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151BE84C-9688-E441-A8A3-A1E4B8C3DCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15980" activeTab="2" xr2:uid="{A7DCC12D-7E8E-1140-B210-C23F3DC9A360}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
     <sheet name="LoginErrorMessage_TC01" sheetId="4" r:id="rId2"/>
-    <sheet name="ForgotPassword4A" sheetId="5" r:id="rId3"/>
+    <sheet name="ForgotPassword4B" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>